<commit_message>
estado civil separado, criar cadastro do conjuge, att whatsapp
</commit_message>
<xml_diff>
--- a/galleriafinancas/src/resource/DashboardTabela.xlsx
+++ b/galleriafinancas/src/resource/DashboardTabela.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Responsável</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Data Cadastro</t>
+  </si>
+  <si>
+    <t>Código</t>
   </si>
 </sst>
 </file>
@@ -480,130 +483,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA15"/>
+  <dimension ref="A1:AB15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="1"/>
-    <col min="15" max="15" width="9.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="39.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="9.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="39.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="3"/>
+      <c r="S1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C2" s="4"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0 #SIS-196# comite no excel do dashboard
</commit_message>
<xml_diff>
--- a/galleriafinancas/src/resource/DashboardTabela.xlsx
+++ b/galleriafinancas/src/resource/DashboardTabela.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Responsável</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>Código</t>
+  </si>
+  <si>
+    <t>Valor Total de Contratos com Boeltos Pagos</t>
+  </si>
+  <si>
+    <t>Aprovadas Comite</t>
+  </si>
+  <si>
+    <t>Valor Total Comite</t>
   </si>
 </sst>
 </file>
@@ -483,44 +492,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB15"/>
+  <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="9.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="39.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="39.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -552,63 +567,69 @@
         <v>6</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>